<commit_message>
LAB4: implemented Api method PUT for updatding records in Car table.
</commit_message>
<xml_diff>
--- a/LAB4/carRest/API_Table.xlsx
+++ b/LAB4/carRest/API_Table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravcz\Desktop\API_REST_JMETER\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravcz\Desktop\TAU_REPO\TAU1\LAB4\carRest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BBC8F6-69C4-4718-A629-2C10FD023C14}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6D602B-08AF-4B28-9567-79C0A6F888D6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1470" yWindow="900" windowWidth="21600" windowHeight="11385" xr2:uid="{DBCD676D-E44F-4CB2-8A78-5759CDD2C089}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -51,12 +51,6 @@
     <t>URL</t>
   </si>
   <si>
-    <t>Display movie with given ID</t>
-  </si>
-  <si>
-    <t>Update info about movie</t>
-  </si>
-  <si>
     <t>Add comment to certain movie ID</t>
   </si>
   <si>
@@ -121,13 +115,34 @@
   </si>
   <si>
     <t>Get all cars</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/test</t>
+  </si>
+  <si>
+    <t>Returns test String</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/car/{id}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/car{id}</t>
+  </si>
+  <si>
+    <t>Get specific car by id</t>
+  </si>
+  <si>
+    <t>Delete car with given id</t>
+  </si>
+  <si>
+    <t>Update Car record with given id by JSON data.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +155,15 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -206,7 +230,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -225,6 +249,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -328,8 +364,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{02A6B254-9104-45FC-B37F-F30166C6BC9F}" name="Tabela1" displayName="Tabela1" ref="A1:D15" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="A1:D15" xr:uid="{8308F36D-2E1F-44CC-B0B3-CCADF6445DF1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{02A6B254-9104-45FC-B37F-F30166C6BC9F}" name="Tabela1" displayName="Tabela1" ref="A1:D17" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="A1:D17" xr:uid="{8308F36D-2E1F-44CC-B0B3-CCADF6445DF1}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{65654B65-90FB-46A9-9698-D0CEBB2943CE}" name="ID" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{D65B1308-7729-48AF-8EBC-BB8D507BA978}" name="METHOD" dataDxfId="2"/>
@@ -637,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825EC626-2FF9-47FC-85CC-2A8DCA89326C}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,211 +703,241 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>29</v>
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>31</v>
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
+      <c r="A4" s="1"/>
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>18</v>
+      <c r="C4" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>18</v>
+        <v>2</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
+        <v>8</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
+        <v>12</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>13</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>14</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>17</v>
+      <c r="C17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{19C30A01-9554-4EA1-8042-0F44333063CA}"/>
-    <hyperlink ref="C15" r:id="rId2" xr:uid="{6A7C0E0E-1167-47EF-9C10-4DF005A72A49}"/>
-    <hyperlink ref="C14" r:id="rId3" xr:uid="{4BC63D51-DB4F-4E34-82A0-D9EA5F349996}"/>
-    <hyperlink ref="C13" r:id="rId4" xr:uid="{0E85F3DD-7A86-4785-B391-52816571361B}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{111B35A7-63A1-4B66-B44C-B23DFA35345C}"/>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{19C30A01-9554-4EA1-8042-0F44333063CA}"/>
+    <hyperlink ref="C17" r:id="rId2" xr:uid="{6A7C0E0E-1167-47EF-9C10-4DF005A72A49}"/>
+    <hyperlink ref="C16" r:id="rId3" xr:uid="{4BC63D51-DB4F-4E34-82A0-D9EA5F349996}"/>
+    <hyperlink ref="C15" r:id="rId4" xr:uid="{0E85F3DD-7A86-4785-B391-52816571361B}"/>
+    <hyperlink ref="C3" r:id="rId5" xr:uid="{111B35A7-63A1-4B66-B44C-B23DFA35345C}"/>
+    <hyperlink ref="C2" r:id="rId6" xr:uid="{04478989-388A-424E-BA4E-4BA2A815414A}"/>
+    <hyperlink ref="C4" r:id="rId7" xr:uid="{6A892CF5-22AC-405A-BC30-82AD9CD3E851}"/>
+    <hyperlink ref="C6" r:id="rId8" xr:uid="{DB1D3867-9F6B-4FC8-9373-ABBD6574583E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
LAB4: adding testPlan with one test: setUp Thread using JDBC to fillup database with records from data.csv file
</commit_message>
<xml_diff>
--- a/LAB4/carRest/API_Table.xlsx
+++ b/LAB4/carRest/API_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravcz\Desktop\TAU_REPO\TAU1\LAB4\carRest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6D602B-08AF-4B28-9567-79C0A6F888D6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B5713A-13B4-4A6E-90EB-2AFC34893585}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="900" windowWidth="21600" windowHeight="11385" xr2:uid="{DBCD676D-E44F-4CB2-8A78-5759CDD2C089}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DBCD676D-E44F-4CB2-8A78-5759CDD2C089}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -51,60 +51,6 @@
     <t>URL</t>
   </si>
   <si>
-    <t>Add comment to certain movie ID</t>
-  </si>
-  <si>
-    <t>Show all comments for givem movie ID</t>
-  </si>
-  <si>
-    <t>Delete certain comment</t>
-  </si>
-  <si>
-    <t>Set Rating of a movie with given ID</t>
-  </si>
-  <si>
-    <t>Add new Actor</t>
-  </si>
-  <si>
-    <t>Show All Actors</t>
-  </si>
-  <si>
-    <t>Add given movie to certain Actor</t>
-  </si>
-  <si>
-    <t>Show actors for certain movie</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/samplerestapp/rest/movies/{id}</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/samplerestapp/rest/movies/{id}/comments</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/samplerestapp/rest/movies/{id}/comments/{commentId}</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/samplerestapp/rest/movies/{id}/ratings</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/samplerestapp/rest/actors</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/samplerestapp/rest/movies/{movieId}/actors</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/samplerestapp/rest/actors/{actorId}/movies</t>
-  </si>
-  <si>
-    <t>Delete a movie with given ID</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/samplerestapp/rest/actors/{actorId}</t>
-  </si>
-  <si>
-    <t>Delete given Actor with certain ID</t>
-  </si>
-  <si>
     <t>http://localhost:8080/api/car</t>
   </si>
   <si>
@@ -135,7 +81,7 @@
     <t>Delete car with given id</t>
   </si>
   <si>
-    <t>Update Car record with given id by JSON data.</t>
+    <t>Update Car record with given id.</t>
   </si>
 </sst>
 </file>
@@ -163,14 +109,14 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,12 +138,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -230,7 +170,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -243,9 +183,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -364,8 +301,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{02A6B254-9104-45FC-B37F-F30166C6BC9F}" name="Tabela1" displayName="Tabela1" ref="A1:D17" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="A1:D17" xr:uid="{8308F36D-2E1F-44CC-B0B3-CCADF6445DF1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{02A6B254-9104-45FC-B37F-F30166C6BC9F}" name="Tabela1" displayName="Tabela1" ref="A1:D7" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="A1:D7" xr:uid="{8308F36D-2E1F-44CC-B0B3-CCADF6445DF1}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{65654B65-90FB-46A9-9698-D0CEBB2943CE}" name="ID" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{D65B1308-7729-48AF-8EBC-BB8D507BA978}" name="METHOD" dataDxfId="2"/>
@@ -673,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825EC626-2FF9-47FC-85CC-2A8DCA89326C}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,239 +642,98 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>31</v>
+      <c r="C2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>27</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
       <c r="B4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>29</v>
+      <c r="C5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>32</v>
+      <c r="C6" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>5</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>6</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>7</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>8</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="C7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>18</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>9</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>10</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>11</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>12</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>13</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>14</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" xr:uid="{19C30A01-9554-4EA1-8042-0F44333063CA}"/>
-    <hyperlink ref="C17" r:id="rId2" xr:uid="{6A7C0E0E-1167-47EF-9C10-4DF005A72A49}"/>
-    <hyperlink ref="C16" r:id="rId3" xr:uid="{4BC63D51-DB4F-4E34-82A0-D9EA5F349996}"/>
-    <hyperlink ref="C15" r:id="rId4" xr:uid="{0E85F3DD-7A86-4785-B391-52816571361B}"/>
-    <hyperlink ref="C3" r:id="rId5" xr:uid="{111B35A7-63A1-4B66-B44C-B23DFA35345C}"/>
-    <hyperlink ref="C2" r:id="rId6" xr:uid="{04478989-388A-424E-BA4E-4BA2A815414A}"/>
-    <hyperlink ref="C4" r:id="rId7" xr:uid="{6A892CF5-22AC-405A-BC30-82AD9CD3E851}"/>
-    <hyperlink ref="C6" r:id="rId8" xr:uid="{DB1D3867-9F6B-4FC8-9373-ABBD6574583E}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{19C30A01-9554-4EA1-8042-0F44333063CA}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{111B35A7-63A1-4B66-B44C-B23DFA35345C}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{04478989-388A-424E-BA4E-4BA2A815414A}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{6A892CF5-22AC-405A-BC30-82AD9CD3E851}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{DB1D3867-9F6B-4FC8-9373-ABBD6574583E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
LAB4: add test for method ureadCar(Integer id)
</commit_message>
<xml_diff>
--- a/LAB4/carRest/API_Table.xlsx
+++ b/LAB4/carRest/API_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravcz\Desktop\TAU_REPO\TAU1\LAB4\carRest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B5713A-13B4-4A6E-90EB-2AFC34893585}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C4A295-0496-440F-99A5-E063006A4947}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DBCD676D-E44F-4CB2-8A78-5759CDD2C089}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>http://localhost:8080/api/car/{id}</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/api/car{id}</t>
   </si>
   <si>
     <t>Get specific car by id</t>
@@ -613,7 +610,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,10 +685,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -705,7 +702,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -719,7 +716,7 @@
         <v>14</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>